<commit_message>
runing tests in the animation
</commit_message>
<xml_diff>
--- a/rawdata/Timetable.xlsx
+++ b/rawdata/Timetable.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Holly\Desktop\rail_simulator\rawdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B513CC-D632-4CD0-8533-91709DD4091E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA0A2E4-FB3F-40F4-9443-5202B0F49E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Timetable" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="277">
   <si>
     <t>ID</t>
   </si>
@@ -101,9 +114,6 @@
   </si>
   <si>
     <t>Start</t>
-  </si>
-  <si>
-    <t>O</t>
   </si>
   <si>
     <t>End</t>
@@ -860,7 +870,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -876,13 +886,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -912,12 +946,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1224,13 +1261,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A322" workbookViewId="0">
-      <selection activeCell="F343" sqref="F343"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="A196" sqref="A196:G203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1250,7 +1289,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -1276,7 +1315,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -1299,7 +1338,7 @@
         <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1322,7 +1361,7 @@
         <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -1345,7 +1384,7 @@
         <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -1362,13 +1401,13 @@
         <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1391,7 +1430,7 @@
         <v>120</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1414,7 +1453,7 @@
         <v>120</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1437,7 +1476,7 @@
         <v>120</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1460,7 +1499,7 @@
         <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1483,7 +1522,7 @@
         <v>90</v>
       </c>
       <c r="G11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1500,13 +1539,13 @@
         <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1529,7 +1568,7 @@
         <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1552,7 +1591,7 @@
         <v>60</v>
       </c>
       <c r="G14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1575,7 +1614,7 @@
         <v>120</v>
       </c>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1592,13 +1631,13 @@
         <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F16">
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1621,7 +1660,7 @@
         <v>60</v>
       </c>
       <c r="G17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1644,7 +1683,7 @@
         <v>60</v>
       </c>
       <c r="G18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1661,13 +1700,13 @@
         <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F19">
         <v>0</v>
       </c>
       <c r="G19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1690,7 +1729,7 @@
         <v>0</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1713,7 +1752,7 @@
         <v>60</v>
       </c>
       <c r="G21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1736,7 +1775,7 @@
         <v>60</v>
       </c>
       <c r="G22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1759,7 +1798,7 @@
         <v>60</v>
       </c>
       <c r="G23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1776,13 +1815,13 @@
         <v>24</v>
       </c>
       <c r="E24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1805,7 +1844,7 @@
         <v>120</v>
       </c>
       <c r="G25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1828,7 +1867,7 @@
         <v>120</v>
       </c>
       <c r="G26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1851,7 +1890,7 @@
         <v>120</v>
       </c>
       <c r="G27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1874,7 +1913,7 @@
         <v>60</v>
       </c>
       <c r="G28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1897,7 +1936,7 @@
         <v>90</v>
       </c>
       <c r="G29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1914,13 +1953,13 @@
         <v>24</v>
       </c>
       <c r="E30" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
       <c r="G30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1943,7 +1982,7 @@
         <v>60</v>
       </c>
       <c r="G31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1966,7 +2005,7 @@
         <v>60</v>
       </c>
       <c r="G32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1989,7 +2028,7 @@
         <v>120</v>
       </c>
       <c r="G33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2006,13 +2045,13 @@
         <v>24</v>
       </c>
       <c r="E34" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F34">
         <v>0</v>
       </c>
       <c r="G34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2035,7 +2074,7 @@
         <v>60</v>
       </c>
       <c r="G35" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -2058,7 +2097,7 @@
         <v>60</v>
       </c>
       <c r="G36" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -2075,13 +2114,13 @@
         <v>24</v>
       </c>
       <c r="E37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F37">
         <v>0</v>
       </c>
       <c r="G37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2104,7 +2143,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2127,7 +2166,7 @@
         <v>60</v>
       </c>
       <c r="G39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2150,7 +2189,7 @@
         <v>60</v>
       </c>
       <c r="G40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -2173,7 +2212,7 @@
         <v>60</v>
       </c>
       <c r="G41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -2190,13 +2229,13 @@
         <v>24</v>
       </c>
       <c r="E42" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F42">
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2219,7 +2258,7 @@
         <v>120</v>
       </c>
       <c r="G43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -2242,7 +2281,7 @@
         <v>120</v>
       </c>
       <c r="G44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -2265,7 +2304,7 @@
         <v>120</v>
       </c>
       <c r="G45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -2288,7 +2327,7 @@
         <v>60</v>
       </c>
       <c r="G46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -2311,7 +2350,7 @@
         <v>90</v>
       </c>
       <c r="G47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -2328,13 +2367,13 @@
         <v>24</v>
       </c>
       <c r="E48" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F48">
         <v>0</v>
       </c>
       <c r="G48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -2357,7 +2396,7 @@
         <v>60</v>
       </c>
       <c r="G49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -2380,7 +2419,7 @@
         <v>60</v>
       </c>
       <c r="G50" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -2403,7 +2442,7 @@
         <v>120</v>
       </c>
       <c r="G51" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -2420,13 +2459,13 @@
         <v>24</v>
       </c>
       <c r="E52" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F52">
         <v>0</v>
       </c>
       <c r="G52" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -2449,7 +2488,7 @@
         <v>60</v>
       </c>
       <c r="G53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -2472,7 +2511,7 @@
         <v>60</v>
       </c>
       <c r="G54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -2489,13 +2528,13 @@
         <v>24</v>
       </c>
       <c r="E55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F55">
         <v>0</v>
       </c>
       <c r="G55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
@@ -2518,7 +2557,7 @@
         <v>0</v>
       </c>
       <c r="G56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
@@ -2541,7 +2580,7 @@
         <v>60</v>
       </c>
       <c r="G57" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
@@ -2564,7 +2603,7 @@
         <v>60</v>
       </c>
       <c r="G58" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
@@ -2587,7 +2626,7 @@
         <v>60</v>
       </c>
       <c r="G59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
@@ -2604,13 +2643,13 @@
         <v>24</v>
       </c>
       <c r="E60" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F60">
         <v>0</v>
       </c>
       <c r="G60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
@@ -2633,7 +2672,7 @@
         <v>120</v>
       </c>
       <c r="G61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
@@ -2656,7 +2695,7 @@
         <v>120</v>
       </c>
       <c r="G62" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
@@ -2679,7 +2718,7 @@
         <v>120</v>
       </c>
       <c r="G63" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
@@ -2702,7 +2741,7 @@
         <v>60</v>
       </c>
       <c r="G64" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
@@ -2725,7 +2764,7 @@
         <v>90</v>
       </c>
       <c r="G65" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -2742,13 +2781,13 @@
         <v>24</v>
       </c>
       <c r="E66" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F66">
         <v>0</v>
       </c>
       <c r="G66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
@@ -2771,7 +2810,7 @@
         <v>60</v>
       </c>
       <c r="G67" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
@@ -2794,7 +2833,7 @@
         <v>60</v>
       </c>
       <c r="G68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
@@ -2817,7 +2856,7 @@
         <v>120</v>
       </c>
       <c r="G69" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
@@ -2834,13 +2873,13 @@
         <v>24</v>
       </c>
       <c r="E70" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F70">
         <v>0</v>
       </c>
       <c r="G70" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
@@ -2863,7 +2902,7 @@
         <v>60</v>
       </c>
       <c r="G71" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -2886,7 +2925,7 @@
         <v>60</v>
       </c>
       <c r="G72" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.3">
@@ -2903,13 +2942,13 @@
         <v>24</v>
       </c>
       <c r="E73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F73">
         <v>0</v>
       </c>
       <c r="G73" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.3">
@@ -2932,7 +2971,7 @@
         <v>0</v>
       </c>
       <c r="G74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.3">
@@ -2955,7 +2994,7 @@
         <v>60</v>
       </c>
       <c r="G75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.3">
@@ -2978,7 +3017,7 @@
         <v>60</v>
       </c>
       <c r="G76" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.3">
@@ -3001,7 +3040,7 @@
         <v>60</v>
       </c>
       <c r="G77" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -3018,13 +3057,13 @@
         <v>24</v>
       </c>
       <c r="E78" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F78">
         <v>0</v>
       </c>
       <c r="G78" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.3">
@@ -3047,7 +3086,7 @@
         <v>120</v>
       </c>
       <c r="G79" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -3070,7 +3109,7 @@
         <v>120</v>
       </c>
       <c r="G80" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.3">
@@ -3093,7 +3132,7 @@
         <v>120</v>
       </c>
       <c r="G81" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.3">
@@ -3116,7 +3155,7 @@
         <v>60</v>
       </c>
       <c r="G82" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.3">
@@ -3139,7 +3178,7 @@
         <v>90</v>
       </c>
       <c r="G83" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -3156,13 +3195,13 @@
         <v>24</v>
       </c>
       <c r="E84" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F84">
         <v>0</v>
       </c>
       <c r="G84" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -3185,7 +3224,7 @@
         <v>60</v>
       </c>
       <c r="G85" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -3208,7 +3247,7 @@
         <v>60</v>
       </c>
       <c r="G86" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
@@ -3231,7 +3270,7 @@
         <v>120</v>
       </c>
       <c r="G87" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -3248,13 +3287,13 @@
         <v>24</v>
       </c>
       <c r="E88" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F88">
         <v>0</v>
       </c>
       <c r="G88" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
@@ -3277,7 +3316,7 @@
         <v>60</v>
       </c>
       <c r="G89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -3300,7 +3339,7 @@
         <v>60</v>
       </c>
       <c r="G90" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.3">
@@ -3317,13 +3356,13 @@
         <v>24</v>
       </c>
       <c r="E91" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F91">
         <v>0</v>
       </c>
       <c r="G91" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.3">
@@ -3346,7 +3385,7 @@
         <v>0</v>
       </c>
       <c r="G92" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.3">
@@ -3369,7 +3408,7 @@
         <v>60</v>
       </c>
       <c r="G93" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.3">
@@ -3392,7 +3431,7 @@
         <v>60</v>
       </c>
       <c r="G94" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.3">
@@ -3415,7 +3454,7 @@
         <v>60</v>
       </c>
       <c r="G95" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -3432,13 +3471,13 @@
         <v>24</v>
       </c>
       <c r="E96" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F96">
         <v>0</v>
       </c>
       <c r="G96" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.3">
@@ -3461,7 +3500,7 @@
         <v>120</v>
       </c>
       <c r="G97" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -3484,7 +3523,7 @@
         <v>120</v>
       </c>
       <c r="G98" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.3">
@@ -3507,7 +3546,7 @@
         <v>120</v>
       </c>
       <c r="G99" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.3">
@@ -3530,7 +3569,7 @@
         <v>60</v>
       </c>
       <c r="G100" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.3">
@@ -3553,7 +3592,7 @@
         <v>90</v>
       </c>
       <c r="G101" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -3570,13 +3609,13 @@
         <v>24</v>
       </c>
       <c r="E102" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F102">
-        <v>0</v>
-      </c>
-      <c r="G102" t="s">
-        <v>33</v>
+        <v>60</v>
+      </c>
+      <c r="G102" s="2">
+        <v>0.71458333333333335</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -3599,7 +3638,7 @@
         <v>60</v>
       </c>
       <c r="G103" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.3">
@@ -3622,7 +3661,7 @@
         <v>60</v>
       </c>
       <c r="G104" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.3">
@@ -3645,7 +3684,7 @@
         <v>120</v>
       </c>
       <c r="G105" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
@@ -3662,13 +3701,13 @@
         <v>24</v>
       </c>
       <c r="E106" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F106">
         <v>0</v>
       </c>
       <c r="G106" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.3">
@@ -3691,7 +3730,7 @@
         <v>60</v>
       </c>
       <c r="G107" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
@@ -3714,7 +3753,7 @@
         <v>60</v>
       </c>
       <c r="G108" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.3">
@@ -3731,13 +3770,13 @@
         <v>24</v>
       </c>
       <c r="E109" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F109">
         <v>0</v>
       </c>
       <c r="G109" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.3">
@@ -3760,7 +3799,7 @@
         <v>0</v>
       </c>
       <c r="G110" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.3">
@@ -3783,7 +3822,7 @@
         <v>60</v>
       </c>
       <c r="G111" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.3">
@@ -3806,7 +3845,7 @@
         <v>60</v>
       </c>
       <c r="G112" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
@@ -3829,7 +3868,7 @@
         <v>60</v>
       </c>
       <c r="G113" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
@@ -3846,13 +3885,13 @@
         <v>24</v>
       </c>
       <c r="E114" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F114">
         <v>0</v>
       </c>
       <c r="G114" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
@@ -3875,7 +3914,7 @@
         <v>120</v>
       </c>
       <c r="G115" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
@@ -3898,7 +3937,7 @@
         <v>120</v>
       </c>
       <c r="G116" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
@@ -3921,7 +3960,7 @@
         <v>120</v>
       </c>
       <c r="G117" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
@@ -3944,7 +3983,7 @@
         <v>60</v>
       </c>
       <c r="G118" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
@@ -3967,7 +4006,7 @@
         <v>90</v>
       </c>
       <c r="G119" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
@@ -3984,13 +4023,13 @@
         <v>24</v>
       </c>
       <c r="E120" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F120">
-        <v>0</v>
-      </c>
-      <c r="G120" t="s">
-        <v>33</v>
+        <v>60</v>
+      </c>
+      <c r="G120" s="2">
+        <v>0.80625000000000002</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
@@ -4013,7 +4052,7 @@
         <v>60</v>
       </c>
       <c r="G121" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
@@ -4036,7 +4075,7 @@
         <v>60</v>
       </c>
       <c r="G122" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
@@ -4059,7 +4098,7 @@
         <v>120</v>
       </c>
       <c r="G123" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.3">
@@ -4076,13 +4115,13 @@
         <v>24</v>
       </c>
       <c r="E124" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F124">
         <v>0</v>
       </c>
       <c r="G124" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.3">
@@ -4105,7 +4144,7 @@
         <v>60</v>
       </c>
       <c r="G125" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
@@ -4128,7 +4167,7 @@
         <v>60</v>
       </c>
       <c r="G126" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
@@ -4145,13 +4184,13 @@
         <v>24</v>
       </c>
       <c r="E127" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F127">
         <v>0</v>
       </c>
       <c r="G127" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
@@ -4174,7 +4213,7 @@
         <v>0</v>
       </c>
       <c r="G128" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
@@ -4197,7 +4236,7 @@
         <v>60</v>
       </c>
       <c r="G129" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
@@ -4220,7 +4259,7 @@
         <v>60</v>
       </c>
       <c r="G130" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
@@ -4243,7 +4282,7 @@
         <v>60</v>
       </c>
       <c r="G131" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
@@ -4260,13 +4299,13 @@
         <v>24</v>
       </c>
       <c r="E132" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F132">
         <v>0</v>
       </c>
       <c r="G132" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
@@ -4289,7 +4328,7 @@
         <v>120</v>
       </c>
       <c r="G133" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
@@ -4312,7 +4351,7 @@
         <v>120</v>
       </c>
       <c r="G134" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
@@ -4335,7 +4374,7 @@
         <v>120</v>
       </c>
       <c r="G135" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
@@ -4358,7 +4397,7 @@
         <v>60</v>
       </c>
       <c r="G136" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
@@ -4381,7 +4420,7 @@
         <v>90</v>
       </c>
       <c r="G137" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
@@ -4398,13 +4437,13 @@
         <v>24</v>
       </c>
       <c r="E138" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F138">
         <v>0</v>
       </c>
       <c r="G138" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
@@ -4427,7 +4466,7 @@
         <v>60</v>
       </c>
       <c r="G139" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
@@ -4450,7 +4489,7 @@
         <v>60</v>
       </c>
       <c r="G140" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
@@ -4473,7 +4512,7 @@
         <v>120</v>
       </c>
       <c r="G141" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
@@ -4490,13 +4529,13 @@
         <v>24</v>
       </c>
       <c r="E142" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F142">
         <v>0</v>
       </c>
       <c r="G142" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
@@ -4519,7 +4558,7 @@
         <v>60</v>
       </c>
       <c r="G143" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
@@ -4542,7 +4581,7 @@
         <v>60</v>
       </c>
       <c r="G144" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.3">
@@ -4559,13 +4598,13 @@
         <v>24</v>
       </c>
       <c r="E145" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F145">
         <v>0</v>
       </c>
       <c r="G145" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.3">
@@ -4588,7 +4627,7 @@
         <v>0</v>
       </c>
       <c r="G146" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.3">
@@ -4611,7 +4650,7 @@
         <v>60</v>
       </c>
       <c r="G147" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.3">
@@ -4634,7 +4673,7 @@
         <v>90</v>
       </c>
       <c r="G148" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.3">
@@ -4651,13 +4690,13 @@
         <v>24</v>
       </c>
       <c r="E149" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F149">
         <v>0</v>
       </c>
       <c r="G149" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.3">
@@ -4680,7 +4719,7 @@
         <v>60</v>
       </c>
       <c r="G150" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.3">
@@ -4703,7 +4742,7 @@
         <v>60</v>
       </c>
       <c r="G151" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.3">
@@ -4726,7 +4765,7 @@
         <v>120</v>
       </c>
       <c r="G152" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.3">
@@ -4743,13 +4782,13 @@
         <v>24</v>
       </c>
       <c r="E153" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F153">
         <v>0</v>
       </c>
       <c r="G153" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.3">
@@ -4772,7 +4811,7 @@
         <v>60</v>
       </c>
       <c r="G154" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.3">
@@ -4795,7 +4834,7 @@
         <v>60</v>
       </c>
       <c r="G155" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.3">
@@ -4812,13 +4851,13 @@
         <v>24</v>
       </c>
       <c r="E156" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F156">
         <v>600</v>
       </c>
       <c r="G156" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.3">
@@ -4841,7 +4880,7 @@
         <v>600</v>
       </c>
       <c r="G157" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.3">
@@ -4864,7 +4903,7 @@
         <v>60</v>
       </c>
       <c r="G158" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.3">
@@ -4887,7 +4926,7 @@
         <v>90</v>
       </c>
       <c r="G159" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.3">
@@ -4904,13 +4943,13 @@
         <v>24</v>
       </c>
       <c r="E160" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F160">
         <v>0</v>
       </c>
       <c r="G160" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.3">
@@ -4933,7 +4972,7 @@
         <v>60</v>
       </c>
       <c r="G161" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.3">
@@ -4956,7 +4995,7 @@
         <v>60</v>
       </c>
       <c r="G162" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.3">
@@ -4979,7 +5018,7 @@
         <v>120</v>
       </c>
       <c r="G163" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.3">
@@ -4996,13 +5035,13 @@
         <v>24</v>
       </c>
       <c r="E164" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F164">
         <v>0</v>
       </c>
       <c r="G164" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.3">
@@ -5025,7 +5064,7 @@
         <v>60</v>
       </c>
       <c r="G165" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.3">
@@ -5048,7 +5087,7 @@
         <v>60</v>
       </c>
       <c r="G166" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.3">
@@ -5065,13 +5104,13 @@
         <v>24</v>
       </c>
       <c r="E167" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F167">
         <v>0</v>
       </c>
       <c r="G167" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.3">
@@ -5094,7 +5133,7 @@
         <v>0</v>
       </c>
       <c r="G168" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.3">
@@ -5117,7 +5156,7 @@
         <v>60</v>
       </c>
       <c r="G169" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.3">
@@ -5140,7 +5179,7 @@
         <v>60</v>
       </c>
       <c r="G170" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.3">
@@ -5157,13 +5196,13 @@
         <v>24</v>
       </c>
       <c r="E171" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F171">
         <v>0</v>
       </c>
       <c r="G171" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.3">
@@ -5186,7 +5225,7 @@
         <v>120</v>
       </c>
       <c r="G172" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.3">
@@ -5209,7 +5248,7 @@
         <v>60</v>
       </c>
       <c r="G173" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.3">
@@ -5231,8 +5270,8 @@
       <c r="F174">
         <v>60</v>
       </c>
-      <c r="G174" t="s">
-        <v>161</v>
+      <c r="G174" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.3">
@@ -5249,13 +5288,13 @@
         <v>24</v>
       </c>
       <c r="E175" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F175">
         <v>0</v>
       </c>
       <c r="G175" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.3">
@@ -5277,8 +5316,8 @@
       <c r="F176">
         <v>120</v>
       </c>
-      <c r="G176" t="s">
-        <v>162</v>
+      <c r="G176" s="3" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.3">
@@ -5301,7 +5340,7 @@
         <v>60</v>
       </c>
       <c r="G177" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.3">
@@ -5324,7 +5363,7 @@
         <v>120</v>
       </c>
       <c r="G178" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.3">
@@ -5347,7 +5386,7 @@
         <v>120</v>
       </c>
       <c r="G179" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
@@ -5370,7 +5409,7 @@
         <v>120</v>
       </c>
       <c r="G180" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
@@ -5387,13 +5426,13 @@
         <v>24</v>
       </c>
       <c r="E181" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F181">
         <v>0</v>
       </c>
       <c r="G181" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
@@ -5415,8 +5454,8 @@
       <c r="F182">
         <v>60</v>
       </c>
-      <c r="G182" t="s">
-        <v>166</v>
+      <c r="G182" s="3" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.3">
@@ -5439,7 +5478,7 @@
         <v>60</v>
       </c>
       <c r="G183" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.3">
@@ -5462,7 +5501,7 @@
         <v>60</v>
       </c>
       <c r="G184" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.3">
@@ -5479,13 +5518,13 @@
         <v>24</v>
       </c>
       <c r="E185" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F185">
         <v>0</v>
       </c>
       <c r="G185" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.3">
@@ -5508,7 +5547,7 @@
         <v>0</v>
       </c>
       <c r="G186" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.3">
@@ -5531,7 +5570,7 @@
         <v>60</v>
       </c>
       <c r="G187" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.3">
@@ -5554,7 +5593,7 @@
         <v>60</v>
       </c>
       <c r="G188" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.3">
@@ -5571,13 +5610,13 @@
         <v>24</v>
       </c>
       <c r="E189" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F189">
         <v>0</v>
       </c>
       <c r="G189" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.3">
@@ -5600,7 +5639,7 @@
         <v>120</v>
       </c>
       <c r="G190" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.3">
@@ -5623,7 +5662,7 @@
         <v>60</v>
       </c>
       <c r="G191" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.3">
@@ -5646,7 +5685,7 @@
         <v>60</v>
       </c>
       <c r="G192" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.3">
@@ -5663,13 +5702,13 @@
         <v>24</v>
       </c>
       <c r="E193" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F193">
         <v>0</v>
       </c>
       <c r="G193" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.3">
@@ -5692,7 +5731,7 @@
         <v>120</v>
       </c>
       <c r="G194" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.3">
@@ -5714,8 +5753,8 @@
       <c r="F195">
         <v>60</v>
       </c>
-      <c r="G195" t="s">
-        <v>175</v>
+      <c r="G195" s="4" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.3">
@@ -5738,7 +5777,7 @@
         <v>120</v>
       </c>
       <c r="G196" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.3">
@@ -5761,7 +5800,7 @@
         <v>120</v>
       </c>
       <c r="G197" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.3">
@@ -5784,7 +5823,7 @@
         <v>120</v>
       </c>
       <c r="G198" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
@@ -5801,13 +5840,13 @@
         <v>24</v>
       </c>
       <c r="E199" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F199">
         <v>0</v>
       </c>
       <c r="G199" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.3">
@@ -5829,8 +5868,8 @@
       <c r="F200">
         <v>60</v>
       </c>
-      <c r="G200" t="s">
-        <v>70</v>
+      <c r="G200" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.3">
@@ -5853,7 +5892,7 @@
         <v>60</v>
       </c>
       <c r="G201" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.3">
@@ -5876,7 +5915,7 @@
         <v>60</v>
       </c>
       <c r="G202" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.3">
@@ -5893,13 +5932,13 @@
         <v>24</v>
       </c>
       <c r="E203" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F203">
         <v>0</v>
       </c>
       <c r="G203" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.3">
@@ -5922,7 +5961,7 @@
         <v>0</v>
       </c>
       <c r="G204" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.3">
@@ -5945,7 +5984,7 @@
         <v>60</v>
       </c>
       <c r="G205" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.3">
@@ -5968,7 +6007,7 @@
         <v>60</v>
       </c>
       <c r="G206" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.3">
@@ -5985,13 +6024,13 @@
         <v>24</v>
       </c>
       <c r="E207" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F207">
         <v>0</v>
       </c>
       <c r="G207" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.3">
@@ -6014,7 +6053,7 @@
         <v>120</v>
       </c>
       <c r="G208" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.3">
@@ -6037,7 +6076,7 @@
         <v>60</v>
       </c>
       <c r="G209" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.3">
@@ -6060,7 +6099,7 @@
         <v>60</v>
       </c>
       <c r="G210" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.3">
@@ -6077,13 +6116,13 @@
         <v>24</v>
       </c>
       <c r="E211" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F211">
         <v>0</v>
       </c>
       <c r="G211" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.3">
@@ -6106,7 +6145,7 @@
         <v>120</v>
       </c>
       <c r="G212" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.3">
@@ -6128,8 +6167,8 @@
       <c r="F213">
         <v>60</v>
       </c>
-      <c r="G213" t="s">
-        <v>186</v>
+      <c r="G213" s="5" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.3">
@@ -6152,7 +6191,7 @@
         <v>120</v>
       </c>
       <c r="G214" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.3">
@@ -6175,7 +6214,7 @@
         <v>120</v>
       </c>
       <c r="G215" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.3">
@@ -6198,7 +6237,7 @@
         <v>120</v>
       </c>
       <c r="G216" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.3">
@@ -6215,13 +6254,13 @@
         <v>24</v>
       </c>
       <c r="E217" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F217">
         <v>0</v>
       </c>
       <c r="G217" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.3">
@@ -6243,8 +6282,8 @@
       <c r="F218">
         <v>60</v>
       </c>
-      <c r="G218" t="s">
-        <v>189</v>
+      <c r="G218" s="5" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.3">
@@ -6267,7 +6306,7 @@
         <v>60</v>
       </c>
       <c r="G219" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.3">
@@ -6290,7 +6329,7 @@
         <v>60</v>
       </c>
       <c r="G220" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.3">
@@ -6307,13 +6346,13 @@
         <v>24</v>
       </c>
       <c r="E221" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F221">
         <v>0</v>
       </c>
       <c r="G221" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.3">
@@ -6336,7 +6375,7 @@
         <v>0</v>
       </c>
       <c r="G222" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.3">
@@ -6359,7 +6398,7 @@
         <v>60</v>
       </c>
       <c r="G223" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.3">
@@ -6382,7 +6421,7 @@
         <v>60</v>
       </c>
       <c r="G224" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.3">
@@ -6399,13 +6438,13 @@
         <v>24</v>
       </c>
       <c r="E225" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F225">
         <v>0</v>
       </c>
       <c r="G225" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.3">
@@ -6428,7 +6467,7 @@
         <v>120</v>
       </c>
       <c r="G226" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.3">
@@ -6451,7 +6490,7 @@
         <v>60</v>
       </c>
       <c r="G227" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.3">
@@ -6474,7 +6513,7 @@
         <v>60</v>
       </c>
       <c r="G228" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.3">
@@ -6491,13 +6530,13 @@
         <v>24</v>
       </c>
       <c r="E229" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F229">
         <v>0</v>
       </c>
       <c r="G229" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.3">
@@ -6520,7 +6559,7 @@
         <v>120</v>
       </c>
       <c r="G230" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.3">
@@ -6543,7 +6582,7 @@
         <v>60</v>
       </c>
       <c r="G231" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.3">
@@ -6566,7 +6605,7 @@
         <v>120</v>
       </c>
       <c r="G232" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.3">
@@ -6589,7 +6628,7 @@
         <v>120</v>
       </c>
       <c r="G233" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.3">
@@ -6612,7 +6651,7 @@
         <v>120</v>
       </c>
       <c r="G234" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.3">
@@ -6629,13 +6668,13 @@
         <v>24</v>
       </c>
       <c r="E235" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F235">
         <v>0</v>
       </c>
       <c r="G235" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.3">
@@ -6658,7 +6697,7 @@
         <v>60</v>
       </c>
       <c r="G236" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.3">
@@ -6681,7 +6720,7 @@
         <v>60</v>
       </c>
       <c r="G237" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.3">
@@ -6704,7 +6743,7 @@
         <v>60</v>
       </c>
       <c r="G238" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.3">
@@ -6721,13 +6760,13 @@
         <v>24</v>
       </c>
       <c r="E239" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F239">
         <v>0</v>
       </c>
       <c r="G239" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.3">
@@ -6750,7 +6789,7 @@
         <v>0</v>
       </c>
       <c r="G240" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.3">
@@ -6773,7 +6812,7 @@
         <v>60</v>
       </c>
       <c r="G241" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.3">
@@ -6796,7 +6835,7 @@
         <v>60</v>
       </c>
       <c r="G242" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.3">
@@ -6813,13 +6852,13 @@
         <v>24</v>
       </c>
       <c r="E243" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F243">
         <v>0</v>
       </c>
       <c r="G243" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.3">
@@ -6842,7 +6881,7 @@
         <v>120</v>
       </c>
       <c r="G244" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.3">
@@ -6865,7 +6904,7 @@
         <v>60</v>
       </c>
       <c r="G245" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="246" spans="1:7" x14ac:dyDescent="0.3">
@@ -6888,7 +6927,7 @@
         <v>60</v>
       </c>
       <c r="G246" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="247" spans="1:7" x14ac:dyDescent="0.3">
@@ -6905,13 +6944,13 @@
         <v>24</v>
       </c>
       <c r="E247" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F247">
         <v>0</v>
       </c>
       <c r="G247" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.3">
@@ -6934,7 +6973,7 @@
         <v>120</v>
       </c>
       <c r="G248" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.3">
@@ -6957,7 +6996,7 @@
         <v>60</v>
       </c>
       <c r="G249" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="250" spans="1:7" x14ac:dyDescent="0.3">
@@ -6980,7 +7019,7 @@
         <v>120</v>
       </c>
       <c r="G250" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="251" spans="1:7" x14ac:dyDescent="0.3">
@@ -7003,7 +7042,7 @@
         <v>120</v>
       </c>
       <c r="G251" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="252" spans="1:7" x14ac:dyDescent="0.3">
@@ -7026,7 +7065,7 @@
         <v>120</v>
       </c>
       <c r="G252" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.3">
@@ -7043,13 +7082,13 @@
         <v>24</v>
       </c>
       <c r="E253" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F253">
         <v>0</v>
       </c>
       <c r="G253" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.3">
@@ -7072,7 +7111,7 @@
         <v>60</v>
       </c>
       <c r="G254" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="255" spans="1:7" x14ac:dyDescent="0.3">
@@ -7095,7 +7134,7 @@
         <v>60</v>
       </c>
       <c r="G255" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.3">
@@ -7118,7 +7157,7 @@
         <v>60</v>
       </c>
       <c r="G256" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.3">
@@ -7135,13 +7174,13 @@
         <v>24</v>
       </c>
       <c r="E257" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F257">
         <v>0</v>
       </c>
       <c r="G257" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.3">
@@ -7164,7 +7203,7 @@
         <v>0</v>
       </c>
       <c r="G258" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.3">
@@ -7187,7 +7226,7 @@
         <v>60</v>
       </c>
       <c r="G259" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.3">
@@ -7210,7 +7249,7 @@
         <v>60</v>
       </c>
       <c r="G260" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.3">
@@ -7227,13 +7266,13 @@
         <v>24</v>
       </c>
       <c r="E261" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F261">
         <v>0</v>
       </c>
       <c r="G261" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.3">
@@ -7256,7 +7295,7 @@
         <v>120</v>
       </c>
       <c r="G262" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.3">
@@ -7279,7 +7318,7 @@
         <v>60</v>
       </c>
       <c r="G263" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.3">
@@ -7302,7 +7341,7 @@
         <v>60</v>
       </c>
       <c r="G264" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.3">
@@ -7319,13 +7358,13 @@
         <v>24</v>
       </c>
       <c r="E265" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F265">
-        <v>0</v>
-      </c>
-      <c r="G265" t="s">
-        <v>33</v>
+        <v>60</v>
+      </c>
+      <c r="G265" s="2">
+        <v>0.71458333333333335</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.3">
@@ -7348,7 +7387,7 @@
         <v>120</v>
       </c>
       <c r="G266" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.3">
@@ -7371,7 +7410,7 @@
         <v>60</v>
       </c>
       <c r="G267" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.3">
@@ -7394,7 +7433,7 @@
         <v>120</v>
       </c>
       <c r="G268" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.3">
@@ -7417,7 +7456,7 @@
         <v>120</v>
       </c>
       <c r="G269" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.3">
@@ -7440,7 +7479,7 @@
         <v>120</v>
       </c>
       <c r="G270" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.3">
@@ -7457,13 +7496,13 @@
         <v>24</v>
       </c>
       <c r="E271" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F271">
         <v>0</v>
       </c>
       <c r="G271" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.3">
@@ -7486,7 +7525,7 @@
         <v>60</v>
       </c>
       <c r="G272" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.3">
@@ -7509,7 +7548,7 @@
         <v>60</v>
       </c>
       <c r="G273" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.3">
@@ -7532,7 +7571,7 @@
         <v>60</v>
       </c>
       <c r="G274" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.3">
@@ -7549,13 +7588,13 @@
         <v>24</v>
       </c>
       <c r="E275" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F275">
         <v>0</v>
       </c>
       <c r="G275" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.3">
@@ -7578,7 +7617,7 @@
         <v>0</v>
       </c>
       <c r="G276" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.3">
@@ -7601,7 +7640,7 @@
         <v>60</v>
       </c>
       <c r="G277" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.3">
@@ -7624,7 +7663,7 @@
         <v>60</v>
       </c>
       <c r="G278" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.3">
@@ -7641,13 +7680,13 @@
         <v>24</v>
       </c>
       <c r="E279" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F279">
         <v>0</v>
       </c>
       <c r="G279" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.3">
@@ -7670,7 +7709,7 @@
         <v>120</v>
       </c>
       <c r="G280" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.3">
@@ -7693,7 +7732,7 @@
         <v>60</v>
       </c>
       <c r="G281" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.3">
@@ -7716,7 +7755,7 @@
         <v>60</v>
       </c>
       <c r="G282" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.3">
@@ -7733,13 +7772,13 @@
         <v>24</v>
       </c>
       <c r="E283" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F283">
         <v>0</v>
       </c>
       <c r="G283" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="284" spans="1:7" x14ac:dyDescent="0.3">
@@ -7762,7 +7801,7 @@
         <v>120</v>
       </c>
       <c r="G284" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.3">
@@ -7785,7 +7824,7 @@
         <v>60</v>
       </c>
       <c r="G285" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.3">
@@ -7808,7 +7847,7 @@
         <v>120</v>
       </c>
       <c r="G286" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.3">
@@ -7831,7 +7870,7 @@
         <v>120</v>
       </c>
       <c r="G287" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.3">
@@ -7854,7 +7893,7 @@
         <v>120</v>
       </c>
       <c r="G288" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.3">
@@ -7871,7 +7910,7 @@
         <v>24</v>
       </c>
       <c r="E289" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F289">
         <v>0</v>
@@ -7897,7 +7936,7 @@
         <v>60</v>
       </c>
       <c r="G290" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.3">
@@ -7920,7 +7959,7 @@
         <v>60</v>
       </c>
       <c r="G291" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.3">
@@ -7943,7 +7982,7 @@
         <v>60</v>
       </c>
       <c r="G292" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.3">
@@ -7960,13 +7999,13 @@
         <v>24</v>
       </c>
       <c r="E293" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F293">
         <v>0</v>
       </c>
       <c r="G293" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.3">
@@ -7989,7 +8028,7 @@
         <v>0</v>
       </c>
       <c r="G294" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="295" spans="1:7" x14ac:dyDescent="0.3">
@@ -8012,7 +8051,7 @@
         <v>60</v>
       </c>
       <c r="G295" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="296" spans="1:7" x14ac:dyDescent="0.3">
@@ -8035,7 +8074,7 @@
         <v>60</v>
       </c>
       <c r="G296" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="297" spans="1:7" x14ac:dyDescent="0.3">
@@ -8052,13 +8091,13 @@
         <v>24</v>
       </c>
       <c r="E297" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F297">
         <v>0</v>
       </c>
       <c r="G297" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.3">
@@ -8081,7 +8120,7 @@
         <v>120</v>
       </c>
       <c r="G298" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.3">
@@ -8104,7 +8143,7 @@
         <v>60</v>
       </c>
       <c r="G299" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="300" spans="1:7" x14ac:dyDescent="0.3">
@@ -8127,7 +8166,7 @@
         <v>60</v>
       </c>
       <c r="G300" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="301" spans="1:7" x14ac:dyDescent="0.3">
@@ -8144,13 +8183,13 @@
         <v>24</v>
       </c>
       <c r="E301" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F301">
         <v>0</v>
       </c>
       <c r="G301" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.3">
@@ -8173,7 +8212,7 @@
         <v>120</v>
       </c>
       <c r="G302" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="303" spans="1:7" x14ac:dyDescent="0.3">
@@ -8196,7 +8235,7 @@
         <v>60</v>
       </c>
       <c r="G303" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.3">
@@ -8213,7 +8252,7 @@
         <v>24</v>
       </c>
       <c r="E304" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F304">
         <v>0</v>
@@ -8242,7 +8281,7 @@
         <v>0</v>
       </c>
       <c r="G305" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="306" spans="1:7" x14ac:dyDescent="0.3">
@@ -8265,7 +8304,7 @@
         <v>60</v>
       </c>
       <c r="G306" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="307" spans="1:7" x14ac:dyDescent="0.3">
@@ -8288,7 +8327,7 @@
         <v>60</v>
       </c>
       <c r="G307" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="308" spans="1:7" x14ac:dyDescent="0.3">
@@ -8305,13 +8344,13 @@
         <v>24</v>
       </c>
       <c r="E308" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F308">
         <v>0</v>
       </c>
       <c r="G308" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="309" spans="1:7" x14ac:dyDescent="0.3">
@@ -8334,7 +8373,7 @@
         <v>120</v>
       </c>
       <c r="G309" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="310" spans="1:7" x14ac:dyDescent="0.3">
@@ -8357,7 +8396,7 @@
         <v>60</v>
       </c>
       <c r="G310" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="311" spans="1:7" x14ac:dyDescent="0.3">
@@ -8380,7 +8419,7 @@
         <v>60</v>
       </c>
       <c r="G311" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="312" spans="1:7" x14ac:dyDescent="0.3">
@@ -8397,13 +8436,13 @@
         <v>24</v>
       </c>
       <c r="E312" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F312">
-        <v>0</v>
-      </c>
-      <c r="G312" t="s">
-        <v>33</v>
+        <v>60</v>
+      </c>
+      <c r="G312" s="2">
+        <v>0.80625000000000002</v>
       </c>
     </row>
     <row r="313" spans="1:7" x14ac:dyDescent="0.3">
@@ -8426,7 +8465,7 @@
         <v>120</v>
       </c>
       <c r="G313" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="314" spans="1:7" x14ac:dyDescent="0.3">
@@ -8449,7 +8488,7 @@
         <v>60</v>
       </c>
       <c r="G314" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="315" spans="1:7" x14ac:dyDescent="0.3">
@@ -8466,13 +8505,13 @@
         <v>24</v>
       </c>
       <c r="E315" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F315">
         <v>0</v>
       </c>
       <c r="G315" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="316" spans="1:7" x14ac:dyDescent="0.3">
@@ -8495,7 +8534,7 @@
         <v>0</v>
       </c>
       <c r="G316" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="317" spans="1:7" x14ac:dyDescent="0.3">
@@ -8518,7 +8557,7 @@
         <v>60</v>
       </c>
       <c r="G317" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="318" spans="1:7" x14ac:dyDescent="0.3">
@@ -8541,7 +8580,7 @@
         <v>60</v>
       </c>
       <c r="G318" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="319" spans="1:7" x14ac:dyDescent="0.3">
@@ -8558,13 +8597,13 @@
         <v>24</v>
       </c>
       <c r="E319" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F319">
         <v>0</v>
       </c>
       <c r="G319" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="320" spans="1:7" x14ac:dyDescent="0.3">
@@ -8587,7 +8626,7 @@
         <v>120</v>
       </c>
       <c r="G320" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="321" spans="1:7" x14ac:dyDescent="0.3">
@@ -8610,7 +8649,7 @@
         <v>60</v>
       </c>
       <c r="G321" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="322" spans="1:7" x14ac:dyDescent="0.3">
@@ -8633,7 +8672,7 @@
         <v>60</v>
       </c>
       <c r="G322" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="323" spans="1:7" x14ac:dyDescent="0.3">
@@ -8650,13 +8689,13 @@
         <v>24</v>
       </c>
       <c r="E323" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F323">
         <v>0</v>
       </c>
       <c r="G323" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="324" spans="1:7" x14ac:dyDescent="0.3">
@@ -8679,7 +8718,7 @@
         <v>120</v>
       </c>
       <c r="G324" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="325" spans="1:7" x14ac:dyDescent="0.3">
@@ -8702,7 +8741,7 @@
         <v>60</v>
       </c>
       <c r="G325" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="326" spans="1:7" x14ac:dyDescent="0.3">
@@ -8725,7 +8764,7 @@
         <v>120</v>
       </c>
       <c r="G326" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="327" spans="1:7" x14ac:dyDescent="0.3">
@@ -8748,7 +8787,7 @@
         <v>120</v>
       </c>
       <c r="G327" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="328" spans="1:7" x14ac:dyDescent="0.3">
@@ -8771,7 +8810,7 @@
         <v>120</v>
       </c>
       <c r="G328" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="329" spans="1:7" x14ac:dyDescent="0.3">
@@ -8788,13 +8827,13 @@
         <v>24</v>
       </c>
       <c r="E329" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F329">
         <v>0</v>
       </c>
       <c r="G329" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="330" spans="1:7" x14ac:dyDescent="0.3">
@@ -8817,7 +8856,7 @@
         <v>60</v>
       </c>
       <c r="G330" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="331" spans="1:7" x14ac:dyDescent="0.3">
@@ -8840,7 +8879,7 @@
         <v>60</v>
       </c>
       <c r="G331" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="332" spans="1:7" x14ac:dyDescent="0.3">
@@ -8863,7 +8902,7 @@
         <v>60</v>
       </c>
       <c r="G332" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="333" spans="1:7" x14ac:dyDescent="0.3">
@@ -8880,13 +8919,13 @@
         <v>24</v>
       </c>
       <c r="E333" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F333">
         <v>0</v>
       </c>
       <c r="G333" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="334" spans="1:7" x14ac:dyDescent="0.3">
@@ -8909,7 +8948,7 @@
         <v>0</v>
       </c>
       <c r="G334" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="335" spans="1:7" x14ac:dyDescent="0.3">
@@ -8932,7 +8971,7 @@
         <v>60</v>
       </c>
       <c r="G335" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="336" spans="1:7" x14ac:dyDescent="0.3">
@@ -8955,7 +8994,7 @@
         <v>60</v>
       </c>
       <c r="G336" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="337" spans="1:7" x14ac:dyDescent="0.3">
@@ -8972,13 +9011,13 @@
         <v>24</v>
       </c>
       <c r="E337" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F337">
         <v>0</v>
       </c>
       <c r="G337" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="338" spans="1:7" x14ac:dyDescent="0.3">
@@ -9001,7 +9040,7 @@
         <v>120</v>
       </c>
       <c r="G338" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="339" spans="1:7" x14ac:dyDescent="0.3">
@@ -9024,7 +9063,7 @@
         <v>60</v>
       </c>
       <c r="G339" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="340" spans="1:7" x14ac:dyDescent="0.3">
@@ -9047,7 +9086,7 @@
         <v>60</v>
       </c>
       <c r="G340" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="341" spans="1:7" x14ac:dyDescent="0.3">
@@ -9064,13 +9103,13 @@
         <v>24</v>
       </c>
       <c r="E341" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F341">
         <v>0</v>
       </c>
       <c r="G341" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="342" spans="1:7" x14ac:dyDescent="0.3">
@@ -9087,7 +9126,7 @@
         <v>24</v>
       </c>
       <c r="E342" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F342">
         <v>0</v>
@@ -9097,6 +9136,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>